<commit_message>
Added exchange qmls and added exchange api call module
</commit_message>
<xml_diff>
--- a/time_template.xlsx
+++ b/time_template.xlsx
@@ -382,7 +382,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\ mmmm"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -442,13 +442,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -456,12 +451,6 @@
       <sz val="9.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1009,7 +998,7 @@
     <xf borderId="18" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="20" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1019,7 +1008,7 @@
     <xf borderId="19" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="19" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="22" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1028,16 +1017,16 @@
     <xf borderId="19" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="22" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="19" fillId="5" fontId="11" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="19" fillId="5" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="23" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="23" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1061,7 +1050,7 @@
     <xf borderId="23" fillId="0" fontId="10" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="23" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="23" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="27" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1086,7 +1075,7 @@
     </xf>
     <xf borderId="40" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="41" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="43" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="44" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -1094,7 +1083,7 @@
     <xf borderId="22" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2453,7 +2442,7 @@
     <row r="43" ht="12.0" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="64" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE("Össz.kötelező munkanap: $1 nap, $2 fiz.ü.nap. (telj.munkaidő össz.óra: $3 óra)", "$1", COUNT(C10:C41)), "$2", E50), "$3", COUNT(C10:C41) * 8)</f>
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE("Össz.kötelező munkanap: $1 nap, $2 fiz.ü.nap. (telj.munkaidő össz.óra: $3 óra)", "$1", COUNT(C10:C40)), "$2", E50), "$3", COUNT(C10:C40) * 8)</f>
         <v>Össz.kötelező munkanap: 31 nap, 0 fiz.ü.nap. (telj.munkaidő össz.óra: 248 óra)</v>
       </c>
       <c r="C43" s="65"/>

</xml_diff>